<commit_message>
Odd channel behaviour for Augist 9 - September 5
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Odd Channel Behavior.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Odd Channel Behavior.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\CIS Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B074BA2E-C6E8-4C4B-8825-9B10C72186B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193F3D1B-4652-427E-ACAE-427E9D943D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8E44477-D6C0-4A59-A814-E37C4647FF29}"/>
+    <workbookView xWindow="2928" yWindow="2988" windowWidth="12948" windowHeight="7944" xr2:uid="{E8E44477-D6C0-4A59-A814-E37C4647FF29}"/>
   </bookViews>
   <sheets>
-    <sheet name="August 2022" sheetId="2" r:id="rId1"/>
-    <sheet name="July 2022" sheetId="1" r:id="rId2"/>
+    <sheet name="September 2022" sheetId="3" r:id="rId1"/>
+    <sheet name="August 2022" sheetId="2" r:id="rId2"/>
+    <sheet name="July 2022" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="153">
   <si>
     <t>EBA</t>
   </si>
@@ -375,13 +376,133 @@
   </si>
   <si>
     <t>Remove bad CIS?  (not in update)</t>
+  </si>
+  <si>
+    <t>Both of these have bad ADC, and there are random runs that are all over the place</t>
+  </si>
+  <si>
+    <t>LBA_m03_c17_lowgain</t>
+  </si>
+  <si>
+    <t>Not in update, but we should ADD Bad CIS, strange downward drift at the end of the month</t>
+  </si>
+  <si>
+    <t>LBA_m14_c37_highgain</t>
+  </si>
+  <si>
+    <t>LBA_m14_c37_lowgain</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>LBA_m35_c08_highgain</t>
+  </si>
+  <si>
+    <t>ADD Bad CIS, strange downward scatter at the end of month</t>
+  </si>
+  <si>
+    <t>DEFAULT, scatter</t>
+  </si>
+  <si>
+    <t>LBC_m01_c25_highgain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad CIS already, similar pattern to odd downward drift in some LBA </t>
+  </si>
+  <si>
+    <t>ADD bad CIS. It's in the update, drift at end of month</t>
+  </si>
+  <si>
+    <t>ADD Bad CIS (not in update, masked) giving inconsistent value as in step function</t>
+  </si>
+  <si>
+    <t>ADD bad CIS (not in update) at end of month there is drift</t>
+  </si>
+  <si>
+    <t>Not in update, half gain</t>
+  </si>
+  <si>
+    <t>LBC_m24_c00-c47_lowgain</t>
+  </si>
+  <si>
+    <t>Recalibrate from end of month (or add bad CIS??) there is a strange outlier point for one of the runs in the middle of the month for all of these, just this moduleand just low gain</t>
+  </si>
+  <si>
+    <t>LBC_m44_c34_highgain</t>
+  </si>
+  <si>
+    <t>Already Bad CIS, some oscillation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: maybe remocve the last two runs </t>
+  </si>
+  <si>
+    <t>LBC_m52_c00-33_lowgain (except c18, c34)</t>
+  </si>
+  <si>
+    <t>At half gain now. Recalibrate from end of month (get rid of plot legend to properly see the remaining points??)</t>
+  </si>
+  <si>
+    <t>This was moved between HG and LG during the month?? Or only one single pon=int for some reason?? Fail Max point in demonstrator</t>
+  </si>
+  <si>
+    <t>Already Bad CIS, slight drift over the course of the month</t>
+  </si>
+  <si>
+    <t>Unusually far from the detector average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EBA_m19_c41_highgain </t>
+  </si>
+  <si>
+    <t>Not in update, ADD Bad CIS due to high scatter,even though somehwat close to detector average</t>
+  </si>
+  <si>
+    <t>Half-gain (not in update)</t>
+  </si>
+  <si>
+    <t>Unusually far from the detector average (not in update)</t>
+  </si>
+  <si>
+    <t>Unusually far from detector average, notin update drift closer to the end of the month</t>
+  </si>
+  <si>
+    <t>Unusually far from detector average (not in update)</t>
+  </si>
+  <si>
+    <t>EBC_m16_c36_lowgain</t>
+  </si>
+  <si>
+    <t>ADD Bad CIS, very far from detector average (not in update)</t>
+  </si>
+  <si>
+    <t>Very far fromdetector average, bad ADC known issue</t>
+  </si>
+  <si>
+    <t>EBC_m20_c10_lowgain</t>
+  </si>
+  <si>
+    <t>Last month seems as though it was bad, but it is now OK -- look into this</t>
+  </si>
+  <si>
+    <t>Bad Cis Calibration due to drifting near beginning of the month; recalibrate channel to end of month values</t>
+  </si>
+  <si>
+    <t>EBC_m56_c41_lowgain</t>
+  </si>
+  <si>
+    <t>Unusually far from detector average (not in update); probably should ADD Bad CIS</t>
+  </si>
+  <si>
+    <t>Unusually far from detector average, step function in the middle of the month, investigate movement of last month (not in update)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +520,23 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -468,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -514,6 +652,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -829,11 +989,391 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A40A11D-3201-4EEC-A05E-A3164E50022C}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="106.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I15" s="21"/>
+    </row>
+    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0386BC-E96B-43FA-B2D4-F7AC885F6095}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,10 +1766,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A862F6-691C-4A02-AB84-51F5BA2160E5}">
   <dimension ref="A1:K19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Odd channel behaviour for November update
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Odd Channel Behavior.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Odd Channel Behavior.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8AE2EB-A6C4-4768-B246-0D4495D0B4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682431C9-C262-454D-811A-7A27CD867FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2988" windowWidth="12948" windowHeight="7944" xr2:uid="{E8E44477-D6C0-4A59-A814-E37C4647FF29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8E44477-D6C0-4A59-A814-E37C4647FF29}"/>
   </bookViews>
   <sheets>
-    <sheet name="September 2022" sheetId="3" r:id="rId1"/>
-    <sheet name="August 2022" sheetId="2" r:id="rId2"/>
-    <sheet name="July 2022" sheetId="1" r:id="rId3"/>
+    <sheet name="November 2022" sheetId="5" r:id="rId1"/>
+    <sheet name="October 2022" sheetId="4" r:id="rId2"/>
+    <sheet name="September 2022" sheetId="3" r:id="rId3"/>
+    <sheet name="August 2022" sheetId="2" r:id="rId4"/>
+    <sheet name="July 2022" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="213">
   <si>
     <t>EBA</t>
   </si>
@@ -496,6 +498,186 @@
   </si>
   <si>
     <t>Unusually far from detector average, step function in the middle of the month, investigate movement of last month (not in update)</t>
+  </si>
+  <si>
+    <t>Unusually far from detector average</t>
+  </si>
+  <si>
+    <t>Drifting down to new plateau</t>
+  </si>
+  <si>
+    <t>Half gain (ADC Affected)</t>
+  </si>
+  <si>
+    <t>EBA_m49_c00_highgain</t>
+  </si>
+  <si>
+    <t>Strange outlier at tge end of the month, bad CIS calibratin anyways</t>
+  </si>
+  <si>
+    <t>EBA_m50_c20_highgain</t>
+  </si>
+  <si>
+    <t>Very far from detector average, looks like there is some shift in the middle of the month (no need to recalibrate at this point)</t>
+  </si>
+  <si>
+    <t>EBA_m61_c15_highgain</t>
+  </si>
+  <si>
+    <t>Recalibrate from 8.9.22. What accounts for the difference?</t>
+  </si>
+  <si>
+    <t>EBC_m16_c36_highgain</t>
+  </si>
+  <si>
+    <t>Change to good CIS calibration, but it is ADC affected anyways, so it won't matter</t>
+  </si>
+  <si>
+    <t>EBC_37_c40_highgain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sridting downwards near the end of the month (not in update </t>
+  </si>
+  <si>
+    <t>Jump in the middle of the month and then returned to normal (future database value will be retained, so it does not matter because it is not really in the update). Make better plots that show the full range for this for the presentaiton</t>
+  </si>
+  <si>
+    <t>LBA_m01_c00-47_highgain</t>
+  </si>
+  <si>
+    <t>Drift up to a stable value, but ADC bad anyways</t>
+  </si>
+  <si>
+    <t>Recalibrate from last two runs of the month.Drifting upwards then slight step function at the end</t>
+  </si>
+  <si>
+    <t>Recalibrate from the last two runs of the month</t>
+  </si>
+  <si>
+    <t>ADD BAD CIS</t>
+  </si>
+  <si>
+    <t>LBC_m20_c37_highgain</t>
+  </si>
+  <si>
+    <t>ADD BAD CIS (not in update)</t>
+  </si>
+  <si>
+    <t>LBC_m20_c37_lowgain</t>
+  </si>
+  <si>
+    <t>LBC_m52_c34_highgain</t>
+  </si>
+  <si>
+    <t>Recalibrate from the end of the month 22.9.22</t>
+  </si>
+  <si>
+    <t>LBC_m52_c34_lowgain</t>
+  </si>
+  <si>
+    <t>Still drifting down, ADC Bad, CIS bad</t>
+  </si>
+  <si>
+    <t>Remove Bad CIS, ADC affected</t>
+  </si>
+  <si>
+    <t>EBA_m39_c31_higgain</t>
+  </si>
+  <si>
+    <t>Beginning of the month is bad, seems to stabilize afterwards. ADC affected anyways</t>
+  </si>
+  <si>
+    <t>EBA_m61_c15_lowgain</t>
+  </si>
+  <si>
+    <t>Previous month's recalibration is remaining stable</t>
+  </si>
+  <si>
+    <t>EBC_m16_c39_highgain</t>
+  </si>
+  <si>
+    <t>Unusually far from detector average (not in update), Bad CIS, ADC affected</t>
+  </si>
+  <si>
+    <t>LBA_m03_c17_highgain</t>
+  </si>
+  <si>
+    <t>Recalibrated, now the channel mean is very far from the detector average yet stable</t>
+  </si>
+  <si>
+    <t>LBA_m06_c40_highgain</t>
+  </si>
+  <si>
+    <t>Far from detector average (not in update), ADC affected anyways</t>
+  </si>
+  <si>
+    <t>LBA_m14_c08_highgain</t>
+  </si>
+  <si>
+    <t>Stable but not at the beginning of the month (should be fine)</t>
+  </si>
+  <si>
+    <t>LBA_m28_c**_**gain</t>
+  </si>
+  <si>
+    <t>Last run in the month it is off (for what reason?), but calibration value will remain the same (green band takes mean as the true mean, not the database-stored one -- this shold be fixed in the plotting code)</t>
+  </si>
+  <si>
+    <t>Masked for what reason?</t>
+  </si>
+  <si>
+    <t>LBA_m30_c15-17,35_**gain</t>
+  </si>
+  <si>
+    <t>LBA_m46_c38_**gain</t>
+  </si>
+  <si>
+    <t>ADC bad, masked anyways</t>
+  </si>
+  <si>
+    <t>Exclude the first two runs of the month</t>
+  </si>
+  <si>
+    <t>LBA_m53_c05_highgain</t>
+  </si>
+  <si>
+    <t>Lowgain is bad, but highgain values seem to systematically underestimate the database values (and for some reason is not in the update)</t>
+  </si>
+  <si>
+    <t>LBA_m63_c**_**gain</t>
+  </si>
+  <si>
+    <t>Last two CIS runs fron 27.10 have it turned off (not in update)</t>
+  </si>
+  <si>
+    <t>Half gain (not in update),high number of failed calibrations</t>
+  </si>
+  <si>
+    <t>LBC_m28_c35_**gain</t>
+  </si>
+  <si>
+    <t>Marked as ADC bad, but CIS calibrations are good</t>
+  </si>
+  <si>
+    <t>LBC_m52_c18_lowgain</t>
+  </si>
+  <si>
+    <t>Good in CIS, but ADC bad, highgain bad</t>
+  </si>
+  <si>
+    <t>LBC_m59_c33_**gain</t>
+  </si>
+  <si>
+    <t>LBC_m62_c08_highgain</t>
+  </si>
+  <si>
+    <t>Recalibrate from third run of the month, bad in Laser, but not really bad in CIS</t>
+  </si>
+  <si>
+    <t>Quite a bit of variation in these channels (still calibration constand is good --&gt; no need to mark as Bad CIS, bit worth reporting)</t>
+  </si>
+  <si>
+    <t>LBC_m63__c24-29, 32-35_**gain</t>
   </si>
 </sst>
 </file>
@@ -606,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -677,6 +859,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -992,11 +1181,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A40A11D-3201-4EEC-A05E-A3164E50022C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839C2A97-A55F-41F1-AEDC-F90081D25840}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,335 +1220,339 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="27" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>113</v>
+        <v>89</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>168</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="27" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="17" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>145</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="27" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="25" t="s">
         <v>114</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>139</v>
+        <v>187</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="27" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="F5" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="27" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="27" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>148</v>
+        <v>153</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="25" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="106.2" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="27" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>140</v>
+        <v>70</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="27" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="27" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="27" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>148</v>
-      </c>
+      <c r="G11" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" s="27" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>200</v>
+      </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>143</v>
-      </c>
+    <row r="13" spans="1:9" s="27" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="F13" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>202</v>
+      </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>149</v>
-      </c>
+    <row r="14" spans="1:9" s="27" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
-      <c r="C15" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>151</v>
-      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="23"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="22" t="s">
-        <v>132</v>
-      </c>
+      <c r="H15" s="22"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
-      <c r="C16" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>152</v>
-      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="23"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
@@ -1373,6 +1566,725 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F4EBE1-C591-4113-B02C-D73845B0A91A}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView topLeftCell="F5" workbookViewId="0">
+      <selection sqref="A1:N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" ht="79.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A40A11D-3201-4EEC-A05E-A3164E50022C}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="106.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0386BC-E96B-43FA-B2D4-F7AC885F6095}">
   <dimension ref="A1:J16"/>
   <sheetViews>
@@ -1774,7 +2686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A862F6-691C-4A02-AB84-51F5BA2160E5}">
   <dimension ref="A1:K19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Recent work update,needs organization
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Odd Channel Behavior.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Odd Channel Behavior.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682431C9-C262-454D-811A-7A27CD867FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2498A633-1E1F-4D86-8A49-8729D096372E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8E44477-D6C0-4A59-A814-E37C4647FF29}"/>
   </bookViews>
@@ -684,7 +684,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,6 +719,24 @@
     <font>
       <sz val="10"/>
       <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -788,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -867,6 +885,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1185,7 +1215,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,10 +1305,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="27" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>179</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -1429,10 +1459,10 @@
       <c r="G9" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1477,10 +1507,10 @@
         <v>153</v>
       </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="32" t="s">
         <v>198</v>
       </c>
       <c r="H11" s="17"/>
@@ -1525,10 +1555,10 @@
       <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" s="27" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="30" t="s">
         <v>183</v>
       </c>
       <c r="C14" s="17"/>

</xml_diff>